<commit_message>
atualização do roteiro de teste
</commit_message>
<xml_diff>
--- a/4.Teste/IFSP_Anote - Roteiro de Teste.xlsx
+++ b/4.Teste/IFSP_Anote - Roteiro de Teste.xlsx
@@ -9,8 +9,10 @@
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
     <sheet name="AUX" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="UCS001" sheetId="3" r:id="rId3"/>
-    <sheet name="UCS002" sheetId="26" r:id="rId4"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Auto Cadastro" sheetId="26" r:id="rId4"/>
+    <sheet name="Caderno" sheetId="29" r:id="rId5"/>
+    <sheet name="Anotacao" sheetId="30" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="___xlfn_IFERROR">NA()</definedName>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
   <si>
     <t>&lt;IFSP_Anote&gt;</t>
   </si>
@@ -62,6 +64,12 @@
   </si>
   <si>
     <t>UC Auto Cadastro</t>
+  </si>
+  <si>
+    <t>UC Caderno</t>
+  </si>
+  <si>
+    <t>UC Anotacao</t>
   </si>
   <si>
     <t>Totais</t>
@@ -208,6 +216,63 @@
     <t>- fetch chamado 1 vez
 - alert não chamado
 - window.location.href permanece como ""</t>
+  </si>
+  <si>
+    <t>Caderno</t>
+  </si>
+  <si>
+    <t>Script de Teste: CadernoServiceTest.java  e CadernoPage.test.jsx</t>
+  </si>
+  <si>
+    <t>Novo caderno</t>
+  </si>
+  <si>
+    <t>Clicar no icone criar caderno e dar um nome</t>
+  </si>
+  <si>
+    <t>Mensagem: ““nome do caderno” criado com sucesso”.</t>
+  </si>
+  <si>
+    <t>Clicar no nome do caderno e na opção de “alterar titulo do caderno”</t>
+  </si>
+  <si>
+    <t>Mensagem “Atualizações salvas com sucesso”.</t>
+  </si>
+  <si>
+    <t>Excluir caderno</t>
+  </si>
+  <si>
+    <t>Clicar no nome do caderno e clicar na opção de excluir</t>
+  </si>
+  <si>
+    <t>Mensagem: “nome do caderno excluido com sucesso”.</t>
+  </si>
+  <si>
+    <t>Novas Anotações</t>
+  </si>
+  <si>
+    <t>Clicar no icone do caderno ou clicar no botão de novas anotações</t>
+  </si>
+  <si>
+    <t>Abrir uma tela para anotações.</t>
+  </si>
+  <si>
+    <t>Salvar anotações</t>
+  </si>
+  <si>
+    <t>Clicar na tela de anotação e na opção de “Salvar anotções”</t>
+  </si>
+  <si>
+    <t>Mensagem “Anotações salvas com sucesso”.</t>
+  </si>
+  <si>
+    <t>Excluir anotações</t>
+  </si>
+  <si>
+    <t>Excluir a anotação sem necessariamente excluir o caderno</t>
+  </si>
+  <si>
+    <t>Mensagem: “certeza que deseja excluir a anotação?”.</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1822,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1839,8 +1904,12 @@
         <v>5</v>
       </c>
       <c r="E5" s="30"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="F5" s="35">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35">
+        <v>0</v>
+      </c>
       <c r="H5" s="35"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
@@ -1856,9 +1925,15 @@
         <v>4</v>
       </c>
       <c r="E6" s="30"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="35">
+        <v>2</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35">
+        <v>0</v>
+      </c>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
@@ -1866,11 +1941,19 @@
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="29"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
+      <c r="C7" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="34">
+        <v>3</v>
+      </c>
       <c r="E7" s="30"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0</v>
+      </c>
       <c r="H7" s="35"/>
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
@@ -1879,10 +1962,16 @@
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="29"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="34">
+        <v>3</v>
+      </c>
       <c r="E8" s="30"/>
-      <c r="F8" s="35"/>
+      <c r="F8" s="35">
+        <v>0</v>
+      </c>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="30"/>
@@ -2036,7 +2125,7 @@
     <row r="20" spans="2:12">
       <c r="B20" s="29"/>
       <c r="C20" s="36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="36"/>
       <c r="E20" s="30"/>
@@ -2052,20 +2141,20 @@
       <c r="B21" s="29"/>
       <c r="C21" s="39">
         <f>COUNTA(C5:C19)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" s="39">
         <f>SUM(D5:D19)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E21" s="30"/>
       <c r="F21" s="40">
         <f>SUM(F5:F19)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="40">
         <f>SUM(G5:G19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="40">
         <f>SUM(H5:H19)</f>
@@ -2073,7 +2162,7 @@
       </c>
       <c r="I21" s="45">
         <f>SUM(F21:H21)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
@@ -2120,17 +2209,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2149,7 +2238,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -2182,7 +2271,7 @@
     </row>
     <row r="3" ht="16.15" customHeight="1" spans="1:254">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2190,7 +2279,7 @@
     </row>
     <row r="4" ht="16.5" customHeight="1" spans="1:254">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -2198,20 +2287,20 @@
     </row>
     <row r="5" ht="16.15" customHeight="1" spans="1:254">
       <c r="A5" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9"/>
       <c r="IT5" s="3"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:254">
       <c r="A6" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="12"/>
       <c r="IT6" s="3"/>
@@ -2219,25 +2308,25 @@
     <row r="7" ht="15" customHeight="1"/>
     <row r="8" ht="15" customHeight="1" spans="1:7">
       <c r="A8" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:23">
@@ -2245,19 +2334,23 @@
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
+      </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -2280,19 +2373,23 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0</v>
+      </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2315,57 +2412,69 @@
         <v>3</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>32</v>
-      </c>
       <c r="E11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+        <v>31</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" ht="16.5" customHeight="1" spans="1:7">
       <c r="A12" s="19">
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" s="47" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" ht="16.5" customHeight="1" spans="1:7">
       <c r="A13" s="19">
         <v>5</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" ht="16.5" customHeight="1" spans="1:7">
       <c r="A14" s="15">
@@ -2455,10 +2564,10 @@
   <sheetPr/>
   <dimension ref="A1:IT19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -2492,7 +2601,7 @@
     </row>
     <row r="3" ht="16.15" customHeight="1" spans="1:254">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2500,7 +2609,7 @@
     </row>
     <row r="4" ht="16.5" customHeight="1" spans="1:254">
       <c r="A4" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -2508,20 +2617,20 @@
     </row>
     <row r="5" ht="16.15" customHeight="1" spans="1:254">
       <c r="A5" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9"/>
       <c r="IT5" s="3"/>
     </row>
     <row r="6" ht="15" customHeight="1" spans="1:254">
       <c r="A6" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6" s="12"/>
       <c r="IT6" s="3"/>
@@ -2529,25 +2638,25 @@
     <row r="7" ht="15" customHeight="1"/>
     <row r="8" ht="15" customHeight="1" spans="1:7">
       <c r="A8" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:23">
@@ -2555,19 +2664,23 @@
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -2590,19 +2703,23 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
+      </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2625,36 +2742,656 @@
         <v>3</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+        <v>31</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" ht="16.5" customHeight="1" spans="1:7">
       <c r="A12" s="19">
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="D12" s="47" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>29</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A13" s="19">
+        <v>5</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A14" s="15">
+        <v>6</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
+        <v>7</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" ht="14.4" spans="1:7">
+      <c r="A16" s="19">
+        <v>8</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="19">
+        <v>9</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="19">
+        <v>10</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="15">
+        <v>11</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:IT19"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="17.8518518518519" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.2222222222222" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.4259259259259" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.5740740740741" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.712962962963" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.1388888888889" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.712962962963" style="2" customWidth="1"/>
+    <col min="8" max="254" width="9.13888888888889" style="2"/>
+    <col min="255" max="16384" width="9.13888888888889" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" spans="1:254">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="IT1" s="3"/>
+    </row>
+    <row r="2" ht="17.4" spans="1:254">
+      <c r="A2" s="5">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="IT2" s="3"/>
+    </row>
+    <row r="3" ht="16.15" customHeight="1" spans="1:254">
+      <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="IT3" s="3"/>
+    </row>
+    <row r="4" ht="16.5" customHeight="1" spans="1:254">
+      <c r="A4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="IT4" s="3"/>
+    </row>
+    <row r="5" ht="16.15" customHeight="1" spans="1:254">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="IT5" s="3"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:254">
+      <c r="A6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="IT6" s="3"/>
+    </row>
+    <row r="7" ht="15" customHeight="1"/>
+    <row r="8" ht="15" customHeight="1" spans="1:7">
+      <c r="A8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="41" customHeight="1" spans="1:23">
+      <c r="A9" s="15">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="32" customHeight="1" spans="1:23">
+      <c r="A10" s="19">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" ht="28" customHeight="1" spans="1:7">
+      <c r="A11" s="19">
+        <v>3</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A12" s="19">
+        <v>4</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A13" s="19">
+        <v>5</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A14" s="15">
+        <v>6</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19">
+        <v>7</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" ht="14.4" spans="1:7">
+      <c r="A16" s="19">
+        <v>8</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="19">
+        <v>9</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="19">
+        <v>10</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="15">
+        <v>11</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:IT19"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="17.8518518518519" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.2222222222222" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.4259259259259" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.5740740740741" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.712962962963" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.1388888888889" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.712962962963" style="2" customWidth="1"/>
+    <col min="8" max="254" width="9.13888888888889" style="2"/>
+    <col min="255" max="16384" width="9.13888888888889" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" spans="1:254">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="IT1" s="3"/>
+    </row>
+    <row r="2" ht="17.4" spans="1:254">
+      <c r="A2" s="5">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="IT2" s="3"/>
+    </row>
+    <row r="3" ht="16.15" customHeight="1" spans="1:254">
+      <c r="A3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="IT3" s="3"/>
+    </row>
+    <row r="4" ht="16.5" customHeight="1" spans="1:254">
+      <c r="A4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="IT4" s="3"/>
+    </row>
+    <row r="5" ht="16.15" customHeight="1" spans="1:254">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="IT5" s="3"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:254">
+      <c r="A6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="IT6" s="3"/>
+    </row>
+    <row r="7" ht="15" customHeight="1"/>
+    <row r="8" ht="15" customHeight="1" spans="1:7">
+      <c r="A8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="35" customHeight="1" spans="1:23">
+      <c r="A9" s="15">
+        <v>1</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="36" customHeight="1" spans="1:23">
+      <c r="A10" s="19">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" ht="42" customHeight="1" spans="1:7">
+      <c r="A11" s="19">
+        <v>3</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" customHeight="1" spans="1:7">
+      <c r="A12" s="19">
+        <v>4</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
     </row>

</xml_diff>